<commit_message>
Implementing ticket #78 :  - This step is able to free/unforce a complete array using its name and path.
</commit_message>
<xml_diff>
--- a/Example/UnitTest 2013 00.xlsx
+++ b/Example/UnitTest 2013 00.xlsx
@@ -11,11 +11,12 @@
     <sheet name="Test_1.2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="59">
   <si>
     <t>Target</t>
   </si>
@@ -141,9 +142,6 @@
   </si>
   <si>
     <t>Unit1/MPU2</t>
-  </si>
-  <si>
-    <t>Unit2/MPU1</t>
   </si>
   <si>
     <t>Unit2/MPU2</t>
@@ -193,6 +191,9 @@
   </si>
   <si>
     <t>Section4/ENV</t>
+  </si>
+  <si>
+    <t>R:Variable[]</t>
   </si>
 </sst>
 </file>
@@ -312,6 +313,9 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="1" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -352,9 +356,6 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -431,10 +432,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_Action_1.1" displayName="Table_Action_1.1" ref="B5:G17" totalsRowCount="1">
-  <autoFilter ref="B5:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_Action_1.1" displayName="Table_Action_1.1" ref="B5:G18" totalsRowCount="1">
+  <autoFilter ref="B5:G17"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="7" totalsRowDxfId="1"/>
     <tableColumn id="2" name="Path"/>
     <tableColumn id="6" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
@@ -446,12 +447,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_Check_1.1" displayName="Table_Check_1.1" ref="B19:G25" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_Check_1.1" displayName="Table_Check_1.1" ref="B20:G26" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" dataDxfId="5"/>
+    <tableColumn id="1" name="Target" dataDxfId="6"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="6" name="Colonne1"/>
-    <tableColumn id="3" name="STEP 1" headerRowDxfId="4"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="5"/>
     <tableColumn id="4" name="Column1"/>
     <tableColumn id="5" name="Column2"/>
   </tableColumns>
@@ -483,10 +484,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:G17" totalsRowCount="1">
-  <autoFilter ref="B5:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:G18" totalsRowCount="1">
+  <autoFilter ref="B5:G17"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="4" totalsRowDxfId="0"/>
     <tableColumn id="2" name="Path"/>
     <tableColumn id="6" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
@@ -498,12 +499,12 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B19:G25" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B20:G26" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" dataDxfId="2"/>
+    <tableColumn id="1" name="Target" dataDxfId="3"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="6" name="Colonne1"/>
-    <tableColumn id="3" name="STEP 1" headerRowDxfId="1"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="2"/>
     <tableColumn id="4" name="Column1"/>
     <tableColumn id="5" name="Column2"/>
   </tableColumns>
@@ -824,10 +825,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D15"/>
+      <selection activeCell="B16" sqref="B16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +864,7 @@
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -904,13 +905,13 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -931,10 +932,10 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -951,7 +952,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E8">
         <v>2000</v>
@@ -971,7 +972,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E9">
         <v>1.5</v>
@@ -991,7 +992,7 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
         <v>33</v>
@@ -1005,7 +1006,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -1019,7 +1020,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1033,7 +1034,7 @@
         <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -1047,7 +1048,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E14">
         <v>-5</v>
@@ -1061,132 +1062,138 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E15">
         <v>-20.8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>16</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19">
-        <v>10</v>
-      </c>
-      <c r="F19">
-        <v>-25</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="42" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22">
-        <v>2.8</v>
-      </c>
-      <c r="F22">
-        <v>-1.7</v>
+      <c r="E22" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="E23">
+        <v>2.8</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>-1.7</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F24">
-        <v>-25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>27</v>
       </c>
-      <c r="D25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25">
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26">
         <v>-1.7</v>
       </c>
     </row>
@@ -1208,10 +1215,10 @@
   <sheetPr codeName="Feuil4">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D25"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1300,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1314,7 +1321,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
         <v>23</v>
@@ -1334,7 +1341,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8">
         <v>2000</v>
@@ -1354,7 +1361,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9">
         <v>1.5</v>
@@ -1374,7 +1381,7 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
         <v>33</v>
@@ -1388,7 +1395,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -1402,7 +1409,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1416,7 +1423,7 @@
         <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -1430,7 +1437,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14">
         <v>-5</v>
@@ -1444,132 +1451,146 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15">
         <v>-20.8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>16</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19">
-        <v>10</v>
-      </c>
-      <c r="F19">
-        <v>-25</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="42" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>38</v>
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22">
-        <v>2.8</v>
-      </c>
-      <c r="F22">
-        <v>-1.7</v>
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="E23">
+        <v>2.8</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>-1.7</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F24">
-        <v>-25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>27</v>
       </c>
-      <c r="D25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25">
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26">
         <v>-1.7</v>
       </c>
     </row>

</xml_diff>